<commit_message>
RNA Practice 1 1.11
</commit_message>
<xml_diff>
--- a/RNA/Practice 1/Resultados.xlsx
+++ b/RNA/Practice 1/Resultados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xvenve/Gits/crispy-invention/RNA/Practice 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324457E9-A6BB-544A-8465-2A06F26ADC8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DF3D17-A822-894C-A52A-E9B9DC6B394B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="5" xr2:uid="{381A8777-1A80-447C-9A6C-76478D5DFAEB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="16800" windowHeight="20500" firstSheet="2" activeTab="5" xr2:uid="{381A8777-1A80-447C-9A6C-76478D5DFAEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos pruebas " sheetId="7" r:id="rId1"/>
@@ -262,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -291,6 +291,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -39575,10 +39576,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C075D4A0-DC5C-427A-8EBF-486DE5B8DC84}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -39588,10 +39589,11 @@
     <col min="3" max="3" width="9.5" customWidth="1"/>
     <col min="4" max="4" width="9.5" style="18" customWidth="1"/>
     <col min="5" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" customWidth="1"/>
+    <col min="10" max="10" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -39613,11 +39615,12 @@
       <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="H1" s="20"/>
+      <c r="J1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>5.0000000000000001E-4</v>
       </c>
@@ -39639,12 +39642,13 @@
       <c r="G2" s="16">
         <v>6.9937269999999999E-3</v>
       </c>
-      <c r="I2" s="17">
+      <c r="H2" s="16"/>
+      <c r="J2" s="17">
         <f>AVERAGE(Tabla132[[#This Row],[E. ENTREN.]:[E. TEST]])</f>
         <v>7.7081836666666667E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0.01</v>
       </c>
@@ -39666,17 +39670,18 @@
       <c r="G3" s="16">
         <v>4.2403349999999996E-3</v>
       </c>
-      <c r="I3" s="17">
+      <c r="H3" s="16"/>
+      <c r="J3" s="17">
         <f>AVERAGE(Tabla132[[#This Row],[E. ENTREN.]:[E. TEST]])</f>
         <v>4.2411303333333332E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0.05</v>
       </c>
       <c r="B4">
-        <v>100000</v>
+        <v>86335</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -39693,17 +39698,18 @@
       <c r="G4" s="16">
         <v>4.401978E-3</v>
       </c>
-      <c r="I4" s="17">
+      <c r="H4" s="16"/>
+      <c r="J4" s="17">
         <f>AVERAGE(Tabla132[[#This Row],[E. ENTREN.]:[E. TEST]])</f>
         <v>3.6482440000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0.75</v>
       </c>
       <c r="B5">
-        <v>100000</v>
+        <v>2987</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -39720,17 +39726,18 @@
       <c r="G5" s="16">
         <v>4.582732E-3</v>
       </c>
-      <c r="I5" s="17">
+      <c r="H5" s="16"/>
+      <c r="J5" s="17">
         <f>AVERAGE(Tabla132[[#This Row],[E. ENTREN.]:[E. TEST]])</f>
         <v>3.6236383333333334E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.1</v>
       </c>
       <c r="B6">
-        <v>100000</v>
+        <v>22927</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -39747,17 +39754,18 @@
       <c r="G6" s="16">
         <v>4.1366839999999998E-3</v>
       </c>
-      <c r="I6" s="17">
+      <c r="H6" s="16"/>
+      <c r="J6" s="17">
         <f>AVERAGE(Tabla132[[#This Row],[E. ENTREN.]:[E. TEST]])</f>
         <v>3.8088383333333333E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.75</v>
       </c>
       <c r="B7">
-        <v>100000</v>
+        <v>4184</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -39774,17 +39782,18 @@
       <c r="G7" s="16">
         <v>3.9561010000000001E-3</v>
       </c>
-      <c r="I7" s="17">
+      <c r="H7" s="16"/>
+      <c r="J7" s="17">
         <f>AVERAGE(Tabla132[[#This Row],[E. ENTREN.]:[E. TEST]])</f>
         <v>3.7199306666666665E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0.75</v>
       </c>
       <c r="B8">
-        <v>100000</v>
+        <v>55718</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -39801,17 +39810,17 @@
       <c r="G8">
         <v>5.0596189999999996E-3</v>
       </c>
-      <c r="I8" s="17">
+      <c r="J8" s="17">
         <f>AVERAGE(Tabla132[[#This Row],[E. ENTREN.]:[E. TEST]])</f>
         <v>3.458001E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0.75</v>
       </c>
       <c r="B9">
-        <v>100000</v>
+        <v>3963</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -39828,17 +39837,17 @@
       <c r="G9">
         <v>4.3019410000000001E-3</v>
       </c>
-      <c r="I9" s="17">
+      <c r="J9" s="17">
         <f>AVERAGE(Tabla132[[#This Row],[E. ENTREN.]:[E. TEST]])</f>
         <v>3.6491953333333336E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0.75</v>
       </c>
       <c r="B10">
-        <v>100000</v>
+        <v>15323</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -39855,17 +39864,17 @@
       <c r="G10">
         <v>6.1128850999999998E-3</v>
       </c>
-      <c r="I10" s="17">
+      <c r="J10" s="17">
         <f>AVERAGE(Tabla132[[#This Row],[E. ENTREN.]:[E. TEST]])</f>
         <v>3.6976111999999996E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0.75</v>
       </c>
       <c r="B11">
-        <v>100000</v>
+        <v>5860</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -39882,17 +39891,17 @@
       <c r="G11">
         <v>3.834652E-3</v>
       </c>
-      <c r="I11" s="17">
+      <c r="J11" s="17">
         <f>AVERAGE(Tabla132[[#This Row],[E. ENTREN.]:[E. TEST]])</f>
         <v>3.1535390000000003E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="B12">
-        <v>1000000</v>
+        <v>938379</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -39909,13 +39918,13 @@
       <c r="G12">
         <v>5.3145650000000003E-3</v>
       </c>
-      <c r="I12" s="17">
+      <c r="J12" s="17">
         <f>AVERAGE(Tabla132[[#This Row],[E. ENTREN.]:[E. TEST]])</f>
         <v>5.0613373333333331E-3</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I2:I12">
+  <conditionalFormatting sqref="J2:J12">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -42546,7 +42555,7 @@
         <v>9.2313444432875105E-2</v>
       </c>
       <c r="D130">
-        <f t="shared" ref="D130:D161" si="8">C130*($E$2-$E$3)+$E$3</f>
+        <f t="shared" ref="D130:D154" si="8">C130*($E$2-$E$3)+$E$3</f>
         <v>9.7399999999999949</v>
       </c>
       <c r="F130">

</xml_diff>